<commit_message>
update: ganti format pengiriman hasil gaji flat
</commit_message>
<xml_diff>
--- a/template/assets/static/FORM-UPLOAD-SLIP-GAJI.xlsx
+++ b/template/assets/static/FORM-UPLOAD-SLIP-GAJI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\kasir\template\assets\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17BAD4A-CA5A-42E9-872B-E0D4495FCF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986CD729-E415-45F3-939B-44A672449054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{687E2A08-6BD6-41BF-A602-15326EBCB938}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{687E2A08-6BD6-41BF-A602-15326EBCB938}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>FORM UPLOAD SLIP GAJI</t>
   </si>
@@ -103,6 +103,66 @@
   </si>
   <si>
     <t>joni.subagyo@email.com</t>
+  </si>
+  <si>
+    <t>GAPOK</t>
+  </si>
+  <si>
+    <t>T. FUNGSIONAL</t>
+  </si>
+  <si>
+    <t>T. KINERJA</t>
+  </si>
+  <si>
+    <t>T. BPJS</t>
+  </si>
+  <si>
+    <t>T. STRUKTURAL</t>
+  </si>
+  <si>
+    <t>T. WALI KELAS</t>
+  </si>
+  <si>
+    <t>T. PENYESUAIAN</t>
+  </si>
+  <si>
+    <t>BPJS</t>
+  </si>
+  <si>
+    <t>Infaq TPP</t>
+  </si>
+  <si>
+    <t>Insijam</t>
+  </si>
+  <si>
+    <t>Kalender</t>
+  </si>
+  <si>
+    <t>Koperasi/Cicilan</t>
+  </si>
+  <si>
+    <t>Lain-lain</t>
+  </si>
+  <si>
+    <t>Pinjaman Bank</t>
+  </si>
+  <si>
+    <t>Pulsa</t>
+  </si>
+  <si>
+    <t>SIMPOK</t>
+  </si>
+  <si>
+    <t>SIMWA</t>
+  </si>
+  <si>
+    <t>Tabungan Wajib</t>
+  </si>
+  <si>
+    <t>Verval SIMPATIKA</t>
+  </si>
+  <si>
+    <t>Verval TPP</t>
   </si>
 </sst>
 </file>
@@ -124,12 +184,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -159,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,6 +251,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7B2E71-B4A2-4D36-B5FB-FCCE661ABF8A}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,9 +587,29 @@
     <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -521,7 +620,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -532,7 +631,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -554,8 +653,68 @@
       <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="H4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="X4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA4" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>21</v>
       </c>
@@ -577,8 +736,68 @@
       <c r="G5" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0</v>
+      </c>
+      <c r="P5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>0</v>
+      </c>
+      <c r="R5" s="8">
+        <v>0</v>
+      </c>
+      <c r="S5" s="8">
+        <v>0</v>
+      </c>
+      <c r="T5" s="8">
+        <v>0</v>
+      </c>
+      <c r="U5" s="8">
+        <v>0</v>
+      </c>
+      <c r="V5" s="8">
+        <v>0</v>
+      </c>
+      <c r="W5" s="8">
+        <v>0</v>
+      </c>
+      <c r="X5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>22</v>
       </c>
@@ -600,8 +819,68 @@
       <c r="G6" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+      <c r="N6" s="8">
+        <v>0</v>
+      </c>
+      <c r="O6" s="8">
+        <v>0</v>
+      </c>
+      <c r="P6" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>0</v>
+      </c>
+      <c r="R6" s="8">
+        <v>0</v>
+      </c>
+      <c r="S6" s="8">
+        <v>0</v>
+      </c>
+      <c r="T6" s="8">
+        <v>0</v>
+      </c>
+      <c r="U6" s="8">
+        <v>0</v>
+      </c>
+      <c r="V6" s="8">
+        <v>0</v>
+      </c>
+      <c r="W6" s="8">
+        <v>0</v>
+      </c>
+      <c r="X6" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>23</v>
       </c>
@@ -623,8 +902,68 @@
       <c r="G7" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="H7" s="8">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0</v>
+      </c>
+      <c r="P7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>0</v>
+      </c>
+      <c r="R7" s="8">
+        <v>0</v>
+      </c>
+      <c r="S7" s="8">
+        <v>0</v>
+      </c>
+      <c r="T7" s="8">
+        <v>0</v>
+      </c>
+      <c r="U7" s="8">
+        <v>0</v>
+      </c>
+      <c r="V7" s="8">
+        <v>0</v>
+      </c>
+      <c r="W7" s="8">
+        <v>0</v>
+      </c>
+      <c r="X7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>24</v>
       </c>
@@ -646,8 +985,68 @@
       <c r="G8" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H8" s="8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0</v>
+      </c>
+      <c r="R8" s="8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="8">
+        <v>0</v>
+      </c>
+      <c r="T8" s="8">
+        <v>0</v>
+      </c>
+      <c r="U8" s="8">
+        <v>0</v>
+      </c>
+      <c r="V8" s="8">
+        <v>0</v>
+      </c>
+      <c r="W8" s="8">
+        <v>0</v>
+      </c>
+      <c r="X8" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>25</v>
       </c>
@@ -668,6 +1067,66 @@
       </c>
       <c r="G9" s="5" t="s">
         <v>10</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>0</v>
+      </c>
+      <c r="N9" s="8">
+        <v>0</v>
+      </c>
+      <c r="O9" s="8">
+        <v>0</v>
+      </c>
+      <c r="P9" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>0</v>
+      </c>
+      <c r="R9" s="8">
+        <v>0</v>
+      </c>
+      <c r="S9" s="8">
+        <v>0</v>
+      </c>
+      <c r="T9" s="8">
+        <v>0</v>
+      </c>
+      <c r="U9" s="8">
+        <v>0</v>
+      </c>
+      <c r="V9" s="8">
+        <v>0</v>
+      </c>
+      <c r="W9" s="8">
+        <v>0</v>
+      </c>
+      <c r="X9" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -677,5 +1136,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>